<commit_message>
commented some code, deleted matplotlib
</commit_message>
<xml_diff>
--- a/data/final_output/Statistic.xlsx
+++ b/data/final_output/Statistic.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chris\Desktop\C++\Covid\data\final_output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D134A89-0551-4E07-B6A5-F806338821BC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E93B68F3-FF13-4C90-9257-FBCEF92B1C68}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17205" yWindow="0" windowWidth="34395" windowHeight="21000" xr2:uid="{B1A6F707-BA90-4212-9CFE-3129C9C7714F}"/>
+    <workbookView xWindow="17205" yWindow="0" windowWidth="17190" windowHeight="21000" xr2:uid="{B1A6F707-BA90-4212-9CFE-3129C9C7714F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,11 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
-  <si>
-    <t>asd</t>
-  </si>
-</sst>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -387,40 +383,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{670B7F24-A120-4C90-A3C9-850F4EFDBDDB}">
-  <dimension ref="E12:E16"/>
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13:E16"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="12" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E12" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E14">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E15">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E16">
-        <v>4</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>